<commit_message>
Cleaning up stuff so we can add new data!
</commit_message>
<xml_diff>
--- a/data/ospree_2019update.xlsx
+++ b/data/ospree_2019update.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28209"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CatherineChamberlain/Documents/git/ospree/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28028"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="2" r:id="rId1"/>
@@ -18,15 +13,15 @@
     <sheet name="data_detailed" sheetId="1" r:id="rId4"/>
     <sheet name="scratch" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -85,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="282">
   <si>
     <t>datasetID</t>
   </si>
@@ -250,9 +245,6 @@
   </si>
   <si>
     <t>Entered By</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-5 letter acronym </t>
   </si>
   <si>
     <t>genus of individual</t>
@@ -571,18 +563,9 @@
     <t>temp.dormancyinduction</t>
   </si>
   <si>
-    <t>fieldsample date</t>
-  </si>
-  <si>
     <t>Budburst Review Meta analysis</t>
   </si>
   <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>From structured search of Web of Science and Google Scholar in 2015</t>
-  </si>
-  <si>
     <t>Name of the pdf or other source material</t>
   </si>
   <si>
@@ -604,9 +587,6 @@
     <t>Pages of journal published</t>
   </si>
   <si>
-    <t>Name of lab member who entered data</t>
-  </si>
-  <si>
     <t>Figures or data tables to scrape from paper</t>
   </si>
   <si>
@@ -712,105 +692,6 @@
     <t>Additional notes</t>
   </si>
   <si>
-    <t>data_simple</t>
-  </si>
-  <si>
-    <t>Extension of 'study', with treatment information filled in for each species / treatment combination</t>
-  </si>
-  <si>
-    <t>species of individual</t>
-  </si>
-  <si>
-    <t>cultivar code</t>
-  </si>
-  <si>
-    <t>name or code of cultivar of individual, if mentioned. Pertains especially to agro-related papers.</t>
-  </si>
-  <si>
-    <t>place of origin of individual, most often found in cross-site studies (e.g. ours: Harvard Forest and St. Hip)</t>
-  </si>
-  <si>
-    <t>Seedling, cutting, potted sapling. The type of material form of the samples studied.</t>
-  </si>
-  <si>
-    <t>Any miscellaneous treatment used in the study: e.g. sugar added to cuttings' water, growth hormone added</t>
-  </si>
-  <si>
-    <t>temp_day</t>
-  </si>
-  <si>
-    <t>"daytime" forcing temperature, C</t>
-  </si>
-  <si>
-    <t>temp_night</t>
-  </si>
-  <si>
-    <t>"nighttime" forcing temperature, C</t>
-  </si>
-  <si>
-    <t>temperature used during any dormancy induction period, C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dormancy induction is a separate process than chilling, and they should be recorded separately. Unless a paper distinctly mentions and tests for "dormancy induction," these columns should not be used. </t>
-  </si>
-  <si>
-    <t>temp_transfer</t>
-  </si>
-  <si>
-    <t>temperature of second chamber/environment if individuals are moved between chambers in study, C</t>
-  </si>
-  <si>
-    <t>daylength_initial</t>
-  </si>
-  <si>
-    <t>original daylength photoperiod if study uses a ramped photoperiod scheme to simulate natural daylength change over time, hours</t>
-  </si>
-  <si>
-    <t>increased by site characteristics</t>
-  </si>
-  <si>
-    <t>Were temperature and photoperiod increased by characteristic values for each site?</t>
-  </si>
-  <si>
-    <t>"daytime" forcing photoperiod, hours</t>
-  </si>
-  <si>
-    <t>"nighttime" forcing photoperiod, hours</t>
-  </si>
-  <si>
-    <t>fieldchill temp</t>
-  </si>
-  <si>
-    <t>temperature of chilling period, C</t>
-  </si>
-  <si>
-    <t>fieldchill photoperiod</t>
-  </si>
-  <si>
-    <t>photoperiod/daylength of chilling period days, hours</t>
-  </si>
-  <si>
-    <t>fieldchill days</t>
-  </si>
-  <si>
-    <t>length of chilling period, days</t>
-  </si>
-  <si>
-    <t>length of freeze treatment, days</t>
-  </si>
-  <si>
-    <t>response variable of scraped data, e.g. daystobudburst, percentbudburst</t>
-  </si>
-  <si>
-    <t>ADDED TO DETAILED</t>
-  </si>
-  <si>
-    <t>was this data added to the data detailed spreadsheet?</t>
-  </si>
-  <si>
-    <t>data_detailed</t>
-  </si>
-  <si>
     <t>Main data sheet. Response variables</t>
   </si>
   <si>
@@ -1019,6 +900,33 @@
   </si>
   <si>
     <t>Publications to extract data from. In Google Drive &gt;&gt; Ospree Papers &gt; Papers_2016_2018</t>
+  </si>
+  <si>
+    <t>From structured search of Web of Science and Google Scholar in 2015 --&gt; Updated in July 2019</t>
+  </si>
+  <si>
+    <t>source tab</t>
+  </si>
+  <si>
+    <t>study tab</t>
+  </si>
+  <si>
+    <t>data_detailed tab</t>
+  </si>
+  <si>
+    <t>your initials (2 or 3 capital letters, no punctuation)</t>
+  </si>
+  <si>
+    <t>Australia, Europe, North America, Cental America, South America, Africa, Asia … or multiple, or leave blank if unclear</t>
+  </si>
+  <si>
+    <t>Name of lab member who entered data (2-3 letters for your initials, no punctuation)</t>
+  </si>
+  <si>
+    <t>Place for quick calculations etc …</t>
+  </si>
+  <si>
+    <t>DO NOT PUT ANYTHING HERE that you want to keep!</t>
   </si>
 </sst>
 </file>
@@ -1028,7 +936,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1085,6 +993,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1103,11 +1026,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1144,14 +1069,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1250,7 +1178,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1302,7 +1230,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1496,7 +1424,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1504,36 +1432,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P160"/>
+  <dimension ref="A1:P125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="24.1640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="88.6640625" customWidth="1"/>
+    <col min="2" max="2" width="60.5" customWidth="1"/>
     <col min="3" max="3" width="58" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="32">
       <c r="A1" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="4" t="s">
-        <v>163</v>
+        <v>274</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>310</v>
+        <v>272</v>
       </c>
       <c r="C4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1541,12 +1469,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16">
       <c r="A7" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B7" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -1559,346 +1487,342 @@
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16">
       <c r="A8" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="13" spans="1:16">
+      <c r="A13" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="14" spans="1:16">
+      <c r="A14" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="16" spans="1:16">
+      <c r="A16" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="17" spans="1:4">
+      <c r="A17" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B17" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="18" spans="1:4">
+      <c r="A18" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B18" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="19" spans="1:4">
+      <c r="A19" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="C19" s="9" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="20" spans="1:4">
+      <c r="B20" s="9" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C20" s="9" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B18" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>180</v>
-      </c>
       <c r="D20" s="9"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="B21" s="9" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="B22" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="D22" s="9"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="D21" s="9"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="9" t="s">
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="D22" s="9"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="4"/>
       <c r="B30" s="6"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B31" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B32" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B33" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B34" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B36" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B32" t="s">
+    <row r="37" spans="1:2">
+      <c r="A37" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B37" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B33" t="s">
+    <row r="38" spans="1:2">
+      <c r="A38" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B38" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B34" t="s">
+    <row r="39" spans="1:2">
+      <c r="A39" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B39" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B35" t="s">
+    <row r="40" spans="1:2">
+      <c r="A40" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B40" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B36" t="s">
+    <row r="41" spans="1:2" ht="32">
+      <c r="A41" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B41" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B37" t="s">
+    <row r="42" spans="1:2">
+      <c r="A42" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B42" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B38" t="s">
+    <row r="43" spans="1:2">
+      <c r="A43" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B43" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B39" t="s">
+    <row r="44" spans="1:2">
+      <c r="A44" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B44" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B40" t="s">
+    <row r="45" spans="1:2">
+      <c r="A45" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B45" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B41" t="s">
+    <row r="46" spans="1:2">
+      <c r="A46" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B46" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B42" t="s">
+    <row r="47" spans="1:2">
+      <c r="A47" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B47" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B43" t="s">
+    <row r="48" spans="1:2">
+      <c r="A48" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B48" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B44" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B45" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B46" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B47" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="B48" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B50" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="4" t="s">
-        <v>208</v>
+        <v>276</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="4"/>
-      <c r="B54" s="6"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" s="3" t="s">
         <v>0</v>
       </c>
@@ -1906,7 +1830,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4">
       <c r="A56" s="3" t="s">
         <v>1</v>
       </c>
@@ -1914,754 +1838,491 @@
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
+    <row r="57" spans="1:4">
+      <c r="A57" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B57" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B58" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="B59" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4">
       <c r="A60" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B60" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B61" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B62" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>62</v>
+      </c>
+      <c r="C63" t="s">
+        <v>66</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B66" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B67" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B62" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" s="3" t="s">
+      <c r="B68" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B74" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B75" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B76" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B77" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B78" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B79" t="s">
+        <v>82</v>
+      </c>
+      <c r="C79" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B80" t="s">
+        <v>85</v>
+      </c>
+      <c r="C80" s="17"/>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B81" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B82" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B83" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B84" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B85" t="s">
+        <v>93</v>
+      </c>
+      <c r="C85" s="17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B86" t="s">
+        <v>96</v>
+      </c>
+      <c r="C86" s="17"/>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B89" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B91" t="s">
         <v>104</v>
       </c>
-      <c r="B63" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="B64" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="B65" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="3" t="s">
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B92" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B93" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B94" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B96" t="s">
         <v>110</v>
       </c>
-      <c r="B66" t="s">
-        <v>220</v>
-      </c>
-      <c r="C66" s="17" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="3" t="s">
+      <c r="C96" s="17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B97" t="s">
+        <v>112</v>
+      </c>
+      <c r="C97" s="19"/>
+    </row>
+    <row r="98" spans="1:3" ht="32">
+      <c r="A98" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B98" t="s">
         <v>113</v>
       </c>
-      <c r="C67" s="17"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="B68" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="B69" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A70" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="B70" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B71" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B72" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="B73" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="B74" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="B75" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="3" t="s">
+      <c r="C98" s="19"/>
+    </row>
+    <row r="99" spans="1:3" ht="32">
+      <c r="A99" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B99" t="s">
+        <v>114</v>
+      </c>
+      <c r="C99" s="19"/>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B100" t="s">
         <v>116</v>
       </c>
-      <c r="B76" t="s">
-        <v>236</v>
-      </c>
-      <c r="C76" s="17" t="s">
+      <c r="C100" s="17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="32">
+      <c r="A101" s="3" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A77" s="3" t="s">
+      <c r="B101" t="s">
         <v>119</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C101" s="17"/>
+    </row>
+    <row r="102" spans="1:3" ht="32">
+      <c r="A102" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C77" s="17"/>
-    </row>
-    <row r="78" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A78" s="3" t="s">
+      <c r="B102" t="s">
         <v>121</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C102" s="17"/>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C78" s="17"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="3" t="s">
+      <c r="B103" t="s">
         <v>123</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C103" s="17"/>
+    </row>
+    <row r="104" spans="1:3" ht="32">
+      <c r="A104" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C79" s="17"/>
-    </row>
-    <row r="80" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A80" s="3" t="s">
+      <c r="B104" t="s">
         <v>125</v>
       </c>
-      <c r="B80" t="s">
-        <v>126</v>
-      </c>
-      <c r="C80" s="17"/>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B82" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B83" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B84" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="B85" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="B88" s="6" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B90" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B91" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B92" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B93" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B94" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B95" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B96" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A97" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B97" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B98" t="s">
-        <v>63</v>
-      </c>
-      <c r="D98" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A99" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B99" t="s">
-        <v>66</v>
-      </c>
-      <c r="C99" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A100" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B100" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A101" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A102" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B102" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A103" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B103" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A104" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B104" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A105" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B105" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A106" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B106" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A107" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B107" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A108" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B108" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A109" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B109" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A110" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B110" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A111" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B111" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A112" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B112" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A113" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B113" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A114" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B114" t="s">
-        <v>83</v>
-      </c>
-      <c r="C114" s="17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A115" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B115" t="s">
-        <v>86</v>
-      </c>
-      <c r="C115" s="17"/>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A116" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B116" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A117" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B117" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A118" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B118" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A119" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B119" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A120" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B120" t="s">
-        <v>94</v>
-      </c>
-      <c r="C120" s="17" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A121" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B121" t="s">
-        <v>97</v>
-      </c>
-      <c r="C121" s="17"/>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A122" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A123" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A124" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B124" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A125" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B125" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A126" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B126" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A127" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B127" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A128" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B128" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A129" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B129" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A130" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A131" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B131" t="s">
-        <v>111</v>
-      </c>
-      <c r="C131" s="17" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A132" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B132" t="s">
-        <v>113</v>
-      </c>
-      <c r="C132" s="18"/>
-    </row>
-    <row r="133" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A133" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B133" t="s">
-        <v>114</v>
-      </c>
-      <c r="C133" s="18"/>
-    </row>
-    <row r="134" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A134" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B134" t="s">
-        <v>115</v>
-      </c>
-      <c r="C134" s="18"/>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A135" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B135" t="s">
-        <v>117</v>
-      </c>
-      <c r="C135" s="17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A136" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B136" t="s">
-        <v>120</v>
-      </c>
-      <c r="C136" s="17"/>
-    </row>
-    <row r="137" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A137" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B137" t="s">
-        <v>122</v>
-      </c>
-      <c r="C137" s="17"/>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A138" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B138" t="s">
-        <v>124</v>
-      </c>
-      <c r="C138" s="17"/>
-    </row>
-    <row r="139" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A139" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B139" t="s">
-        <v>126</v>
-      </c>
-      <c r="C139" s="17"/>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A142" s="10"/>
-      <c r="B142" s="11"/>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A143" s="11"/>
-      <c r="B143" s="11"/>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A144" s="11"/>
-      <c r="B144" s="11"/>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" s="10"/>
-      <c r="B145" s="11"/>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A146" s="12"/>
-      <c r="B146" s="11"/>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A147" s="10"/>
-      <c r="B147" s="11"/>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A148" s="10"/>
-      <c r="B148" s="11"/>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A149" s="10"/>
-      <c r="B149" s="11"/>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A150" s="10"/>
-      <c r="B150" s="11"/>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A151" s="10"/>
-      <c r="B151" s="11"/>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A152" s="19"/>
-      <c r="B152" s="19"/>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A153" s="13"/>
-      <c r="B153" s="14"/>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A154" s="10"/>
-      <c r="B154" s="11"/>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A155" s="10"/>
-      <c r="B155" s="11"/>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A156" s="10"/>
-      <c r="B156" s="11"/>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A157" s="10"/>
-      <c r="B157" s="11"/>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A158" s="10"/>
-      <c r="B158" s="11"/>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A159" s="10"/>
-      <c r="B159" s="11"/>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A160" s="10"/>
-      <c r="B160" s="11"/>
+      <c r="C104" s="17"/>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="10"/>
+      <c r="B107" s="11"/>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="11"/>
+      <c r="B108" s="11"/>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="11"/>
+      <c r="B109" s="11"/>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="10"/>
+      <c r="B110" s="11"/>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" s="12"/>
+      <c r="B111" s="11"/>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="10"/>
+      <c r="B112" s="11"/>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="10"/>
+      <c r="B113" s="11"/>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="10"/>
+      <c r="B114" s="11"/>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="10"/>
+      <c r="B115" s="11"/>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="10"/>
+      <c r="B116" s="11"/>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" s="18"/>
+      <c r="B117" s="18"/>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" s="13"/>
+      <c r="B118" s="14"/>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="10"/>
+      <c r="B119" s="11"/>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="10"/>
+      <c r="B120" s="11"/>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" s="10"/>
+      <c r="B121" s="11"/>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="10"/>
+      <c r="B122" s="11"/>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="10"/>
+      <c r="B123" s="11"/>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="10"/>
+      <c r="B124" s="11"/>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="10"/>
+      <c r="B125" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="C135:C139"/>
-    <mergeCell ref="A152:B152"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="C76:C80"/>
-    <mergeCell ref="C114:C115"/>
-    <mergeCell ref="C120:C121"/>
-    <mergeCell ref="C131:C134"/>
+  <mergeCells count="5">
+    <mergeCell ref="C100:C104"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="C96:C99"/>
   </mergeCells>
   <conditionalFormatting sqref="A7">
     <cfRule type="containsBlanks" dxfId="3" priority="2">
@@ -2674,9 +2335,15 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D98" r:id="rId1"/>
+    <hyperlink ref="D63" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2685,375 +2352,376 @@
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="S1" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
-        <v>248</v>
+        <v>210</v>
       </c>
       <c r="B2" t="s">
-        <v>242</v>
+        <v>204</v>
       </c>
       <c r="C2" t="s">
-        <v>243</v>
+        <v>205</v>
       </c>
       <c r="D2">
         <v>2019</v>
       </c>
       <c r="E2" t="s">
-        <v>244</v>
+        <v>206</v>
       </c>
       <c r="F2" t="s">
-        <v>245</v>
+        <v>207</v>
       </c>
       <c r="G2">
         <v>25</v>
       </c>
       <c r="H2" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>247</v>
+        <v>209</v>
       </c>
       <c r="B3" t="s">
-        <v>278</v>
+        <v>240</v>
       </c>
       <c r="C3" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
       <c r="D3">
         <v>2017</v>
       </c>
       <c r="E3" t="s">
-        <v>280</v>
+        <v>242</v>
       </c>
       <c r="F3" t="s">
-        <v>281</v>
+        <v>243</v>
       </c>
       <c r="G3">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
-        <v>249</v>
+        <v>211</v>
       </c>
       <c r="B4" t="s">
-        <v>305</v>
+        <v>267</v>
       </c>
       <c r="C4" t="s">
-        <v>306</v>
+        <v>268</v>
       </c>
       <c r="D4">
         <v>2108</v>
       </c>
       <c r="E4" t="s">
-        <v>307</v>
+        <v>269</v>
       </c>
       <c r="F4" t="s">
-        <v>308</v>
+        <v>270</v>
       </c>
       <c r="G4">
         <v>560</v>
       </c>
       <c r="H4" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>250</v>
+        <v>212</v>
       </c>
       <c r="B5" t="s">
-        <v>301</v>
+        <v>263</v>
       </c>
       <c r="C5" t="s">
-        <v>302</v>
+        <v>264</v>
       </c>
       <c r="D5">
         <v>2017</v>
       </c>
       <c r="E5" t="s">
-        <v>303</v>
+        <v>265</v>
       </c>
       <c r="F5" t="s">
-        <v>260</v>
+        <v>222</v>
       </c>
       <c r="G5">
         <v>216</v>
       </c>
       <c r="H5" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>251</v>
+        <v>213</v>
       </c>
       <c r="B6" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="C6" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="D6">
         <v>2018</v>
       </c>
       <c r="E6" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F6" t="s">
-        <v>295</v>
+        <v>257</v>
       </c>
       <c r="H6" s="16"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
-        <v>252</v>
+        <v>214</v>
       </c>
       <c r="B7" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
       <c r="C7" t="s">
-        <v>258</v>
+        <v>220</v>
       </c>
       <c r="D7">
         <v>2018</v>
       </c>
       <c r="E7" t="s">
-        <v>259</v>
+        <v>221</v>
       </c>
       <c r="F7" t="s">
-        <v>260</v>
+        <v>222</v>
       </c>
       <c r="G7">
         <v>219</v>
       </c>
       <c r="H7" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
-        <v>253</v>
+        <v>215</v>
       </c>
       <c r="B8" t="s">
-        <v>273</v>
+        <v>235</v>
       </c>
       <c r="C8" t="s">
-        <v>274</v>
+        <v>236</v>
       </c>
       <c r="D8">
         <v>2018</v>
       </c>
       <c r="E8" t="s">
-        <v>275</v>
+        <v>237</v>
       </c>
       <c r="F8" t="s">
-        <v>276</v>
+        <v>238</v>
       </c>
       <c r="G8">
         <v>248</v>
       </c>
       <c r="H8" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="B9" t="s">
-        <v>296</v>
+        <v>258</v>
       </c>
       <c r="C9" t="s">
-        <v>297</v>
+        <v>259</v>
       </c>
       <c r="D9">
         <v>2017</v>
       </c>
       <c r="E9" t="s">
-        <v>298</v>
+        <v>260</v>
       </c>
       <c r="F9" t="s">
-        <v>299</v>
+        <v>261</v>
       </c>
       <c r="G9">
         <v>37</v>
       </c>
       <c r="H9" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
-        <v>255</v>
+        <v>217</v>
       </c>
       <c r="B10" t="s">
-        <v>282</v>
+        <v>244</v>
       </c>
       <c r="C10" t="s">
-        <v>283</v>
+        <v>245</v>
       </c>
       <c r="D10">
         <v>2016</v>
       </c>
       <c r="E10" t="s">
-        <v>284</v>
+        <v>246</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>285</v>
+        <v>247</v>
       </c>
       <c r="G10">
         <v>37</v>
       </c>
       <c r="H10" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
       <c r="B11" t="s">
-        <v>287</v>
+        <v>249</v>
       </c>
       <c r="C11" t="s">
-        <v>288</v>
+        <v>250</v>
       </c>
       <c r="D11">
         <v>2018</v>
       </c>
       <c r="E11" t="s">
-        <v>289</v>
+        <v>251</v>
       </c>
       <c r="F11" t="s">
-        <v>290</v>
+        <v>252</v>
       </c>
       <c r="G11">
         <v>42</v>
       </c>
       <c r="H11" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" t="s">
-        <v>257</v>
+        <v>219</v>
       </c>
       <c r="B12" t="s">
-        <v>268</v>
+        <v>230</v>
       </c>
       <c r="C12" t="s">
-        <v>269</v>
+        <v>231</v>
       </c>
       <c r="D12">
         <v>2018</v>
       </c>
       <c r="E12" t="s">
-        <v>270</v>
+        <v>232</v>
       </c>
       <c r="F12" t="s">
-        <v>271</v>
+        <v>233</v>
       </c>
       <c r="G12">
         <v>231</v>
       </c>
       <c r="H12" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" t="s">
-        <v>262</v>
+        <v>224</v>
       </c>
       <c r="B13" t="s">
-        <v>263</v>
+        <v>225</v>
       </c>
       <c r="C13" t="s">
-        <v>265</v>
+        <v>227</v>
       </c>
       <c r="D13">
         <v>2018</v>
       </c>
       <c r="E13" t="s">
-        <v>266</v>
+        <v>228</v>
       </c>
       <c r="F13" t="s">
-        <v>245</v>
+        <v>207</v>
       </c>
       <c r="G13">
         <v>24</v>
       </c>
       <c r="H13" t="s">
-        <v>267</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -3069,6 +2737,11 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3077,75 +2750,81 @@
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:20" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="6" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="7" t="s">
         <v>159</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>160</v>
       </c>
       <c r="S1" s="6" t="s">
         <v>7</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3157,9 +2836,9 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:53" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3322,172 +3001,40 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I1" t="s">
-        <v>62</v>
-      </c>
-      <c r="J1" t="s">
-        <v>65</v>
-      </c>
-      <c r="K1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" t="s">
-        <v>18</v>
-      </c>
-      <c r="S1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T1" t="s">
-        <v>20</v>
-      </c>
-      <c r="U1" t="s">
-        <v>21</v>
-      </c>
-      <c r="V1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W1" t="s">
-        <v>23</v>
-      </c>
-      <c r="X1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>99</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>110</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>116</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>119</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>121</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>123</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>125</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>96</v>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="20" t="s">
+        <v>281</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updating who did what new papers
</commit_message>
<xml_diff>
--- a/data/ospree_2019update.xlsx
+++ b/data/ospree_2019update.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20980" yWindow="5660" windowWidth="25600" windowHeight="14240" activeTab="1"/>
+    <workbookView xWindow="10760" yWindow="5500" windowWidth="25600" windowHeight="14240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="2" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="297">
   <si>
     <t>datasetID</t>
   </si>
@@ -966,6 +966,12 @@
   </si>
   <si>
     <t>Who’s who? Initials</t>
+  </si>
+  <si>
+    <t>EMW</t>
+  </si>
+  <si>
+    <t>KL to check</t>
   </si>
 </sst>
 </file>
@@ -1065,9 +1071,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1118,12 +1125,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1468,7 +1476,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2425,7 +2433,7 @@
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2521,6 +2529,9 @@
       <c r="J2" t="s">
         <v>284</v>
       </c>
+      <c r="L2" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
@@ -2576,6 +2587,9 @@
       <c r="J4" t="s">
         <v>282</v>
       </c>
+      <c r="L4" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" t="s">
@@ -2656,7 +2670,7 @@
         <v>223</v>
       </c>
       <c r="J7" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -2685,7 +2699,7 @@
         <v>239</v>
       </c>
       <c r="J8" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="9" spans="1:19">

</xml_diff>

<commit_message>
Added who should review others work!
</commit_message>
<xml_diff>
--- a/data/ospree_2019update.xlsx
+++ b/data/ospree_2019update.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10760" yWindow="5500" windowWidth="25600" windowHeight="14240" activeTab="1"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="2" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="301">
   <si>
     <t>datasetID</t>
   </si>
@@ -972,6 +972,18 @@
   </si>
   <si>
     <t>KL to check</t>
+  </si>
+  <si>
+    <t>CC to check</t>
+  </si>
+  <si>
+    <t>DB to check</t>
+  </si>
+  <si>
+    <t>DL to check</t>
+  </si>
+  <si>
+    <t>DS to check</t>
   </si>
 </sst>
 </file>
@@ -1071,9 +1083,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1125,13 +1139,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="10">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1476,7 +1492,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2433,7 +2449,7 @@
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2558,6 +2574,9 @@
       <c r="J3" t="s">
         <v>285</v>
       </c>
+      <c r="L3" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" t="s">
@@ -2619,6 +2638,9 @@
       <c r="J5" t="s">
         <v>287</v>
       </c>
+      <c r="L5" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
@@ -2643,6 +2665,9 @@
       <c r="J6" t="s">
         <v>287</v>
       </c>
+      <c r="L6" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" t="s">
@@ -2672,6 +2697,9 @@
       <c r="J7" t="s">
         <v>295</v>
       </c>
+      <c r="L7" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" t="s">
@@ -2701,6 +2729,9 @@
       <c r="J8" t="s">
         <v>285</v>
       </c>
+      <c r="L8" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" t="s">
@@ -2730,6 +2761,9 @@
       <c r="J9" t="s">
         <v>286</v>
       </c>
+      <c r="L9" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" t="s">
@@ -2759,6 +2793,9 @@
       <c r="J10" t="s">
         <v>286</v>
       </c>
+      <c r="L10" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" t="s">
@@ -2788,6 +2825,9 @@
       <c r="J11" t="s">
         <v>286</v>
       </c>
+      <c r="L11" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" t="s">
@@ -2817,6 +2857,9 @@
       <c r="J12" t="s">
         <v>286</v>
       </c>
+      <c r="L12" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" t="s">
@@ -2845,6 +2888,9 @@
       </c>
       <c r="J13" t="s">
         <v>283</v>
+      </c>
+      <c r="L13" t="s">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>